<commit_message>
Simplificação da primeira implementação, mesmo resultado.
</commit_message>
<xml_diff>
--- a/grafo_analise.xlsx
+++ b/grafo_analise.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alemao\Documents\Ubots\TesteAdmissionalPraticoUbots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31A20DCB-6D69-4AC1-A83B-3CDB7ACDAB44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DA2A6B-E1CB-4410-863D-F83C01A484CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grafo_analise" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -295,7 +303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +620,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -773,8 +787,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1129,11 +1144,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AO300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AO300"/>
+    <sheetView tabSelected="1" topLeftCell="D276" workbookViewId="0">
+      <selection activeCell="Q300" sqref="Q300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25004,7 +25019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>65</v>
       </c>
@@ -25093,7 +25108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>64</v>
       </c>
@@ -25182,7 +25197,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>63</v>
       </c>
@@ -25271,12 +25286,130 @@
         <v>16</v>
       </c>
     </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B260">
+        <f>SUM(B233:B259)</f>
+        <v>5</v>
+      </c>
+      <c r="C260">
+        <f t="shared" ref="C260:AB260" si="0">SUM(C233:C259)</f>
+        <v>5</v>
+      </c>
+      <c r="D260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E260">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F260">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L260">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="M260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="O260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R260">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="S260">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="T260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="U260">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="V260">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="W260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="X260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Y260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Z260">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AA260">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AB260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AC260">
+        <f>SUM(B260:AB260)</f>
+        <v>225</v>
+      </c>
+      <c r="AD260">
+        <f>AC260/25</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="261" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>16</v>
       </c>
@@ -25344,7 +25477,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="263" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>69</v>
       </c>
@@ -25412,7 +25545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>42</v>
       </c>
@@ -25480,7 +25613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>52</v>
       </c>
@@ -25548,7 +25681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>55</v>
       </c>
@@ -25616,7 +25749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>72</v>
       </c>
@@ -25684,7 +25817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="268" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>45</v>
       </c>
@@ -25752,7 +25885,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>59</v>
       </c>
@@ -25820,7 +25953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>83</v>
       </c>
@@ -25888,7 +26021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>57</v>
       </c>
@@ -25956,7 +26089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>75</v>
       </c>
@@ -26909,7 +27042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>43</v>
       </c>
@@ -26959,7 +27092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>44</v>
       </c>
@@ -27009,7 +27142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>45</v>
       </c>
@@ -27059,7 +27192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>83</v>
       </c>
@@ -27109,7 +27242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>46</v>
       </c>
@@ -27159,7 +27292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>47</v>
       </c>
@@ -27209,7 +27342,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>60</v>
       </c>
@@ -27259,7 +27392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>48</v>
       </c>
@@ -27309,7 +27442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>49</v>
       </c>
@@ -27359,7 +27492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>50</v>
       </c>
@@ -27409,7 +27542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>65</v>
       </c>
@@ -27457,6 +27590,71 @@
       </c>
       <c r="P299" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="300" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B300" s="1">
+        <f>SUM(B286:B299)</f>
+        <v>10</v>
+      </c>
+      <c r="C300" s="1">
+        <f t="shared" ref="C300:O300" si="1">SUM(C286:C299)</f>
+        <v>10</v>
+      </c>
+      <c r="D300" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E300" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F300" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G300" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H300" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I300" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J300" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K300" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L300" s="1">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="M300" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N300" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O300" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P300" s="1">
+        <f>SUM(B300:O300)</f>
+        <v>125</v>
+      </c>
+      <c r="Q300">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>